<commit_message>
update relatorio_financeiro.xlsx with new financial data
</commit_message>
<xml_diff>
--- a/relatorio_financeiro.xlsx
+++ b/relatorio_financeiro.xlsx
@@ -16,7 +16,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;R$&quot;#,##0.00"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -27,17 +29,23 @@
     </font>
     <font>
       <b val="1"/>
+      <color rgb="00FFFFFF"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="004F81BD"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -45,13 +53,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -160,12 +177,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Relatório Financeiro'!$A$2:$A$8</f>
+              <f>'Relatório Financeiro'!$A$2:$A$6</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Relatório Financeiro'!$B$2:$B$8</f>
+              <f>'Relatório Financeiro'!$B$2:$B$6</f>
             </numRef>
           </val>
         </ser>
@@ -521,13 +538,18 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="17" customWidth="1" min="1" max="1"/>
+    <col width="13" customWidth="1" min="2" max="2"/>
+    <col width="15" customWidth="1" min="3" max="3"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -552,7 +574,7 @@
           <t>Salário</t>
         </is>
       </c>
-      <c r="B2" t="n">
+      <c r="B2" s="2" t="n">
         <v>5000</v>
       </c>
       <c r="C2" t="inlineStr">
@@ -567,8 +589,8 @@
           <t>Renda extra</t>
         </is>
       </c>
-      <c r="B3" t="n">
-        <v>200</v>
+      <c r="B3" s="2" t="n">
+        <v>300</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -582,56 +604,34 @@
           <t>teste1</t>
         </is>
       </c>
-      <c r="B4" t="n">
-        <v>200</v>
+      <c r="B4" s="2" t="n">
+        <v>304</v>
       </c>
       <c r="C4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>teste2</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>300</v>
+          <t>Total de gastos</t>
+        </is>
+      </c>
+      <c r="B5" s="2">
+        <f>SUM(B4:B4)</f>
+        <v/>
       </c>
       <c r="C5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>teste3</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>23</v>
+          <t>Saldo final</t>
+        </is>
+      </c>
+      <c r="B6" s="2">
+        <f>B2+B3-B5</f>
+        <v/>
       </c>
       <c r="C6" t="inlineStr"/>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Total de gastos</t>
-        </is>
-      </c>
-      <c r="B7">
-        <f>SUM(B4:B6)</f>
-        <v/>
-      </c>
-      <c r="C7" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Saldo final</t>
-        </is>
-      </c>
-      <c r="B8">
-        <f>B2+B3-B7</f>
-        <v/>
-      </c>
-      <c r="C8" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>